<commit_message>
Fade out for splash
</commit_message>
<xml_diff>
--- a/doc/organisation/Burndown Chart/Sprint 4.xlsx
+++ b/doc/organisation/Burndown Chart/Sprint 4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patigny.nicolas\AndroidStudioProjects\BSN_2024\doc\organisation\Burndown Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A1D3B4-13C1-445E-A219-0580B805F8B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662941F9-3C1B-45DF-898F-EEB66D6F5ADE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>Initial Estimate</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>US#5 API:Al</t>
+  </si>
+  <si>
+    <t>0.5</t>
   </si>
 </sst>
 </file>
@@ -294,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -313,6 +316,18 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,7 +802,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1037,67 +1052,67 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2497,7 +2512,7 @@
   <dimension ref="A1:AN13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2638,30 +2653,32 @@
       <c r="I2" s="5">
         <v>5</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
+      <c r="J2" s="19">
+        <v>2</v>
+      </c>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
       <c r="AE2" s="8">
         <f>B2-(SUM(C2:AD2))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.35">
@@ -2692,27 +2709,29 @@
       <c r="I3" s="6">
         <v>2</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
+      <c r="J3" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="18"/>
       <c r="AE3" s="9">
         <f>B3-(SUM(C3:AD3))</f>
         <v>4</v>
@@ -2746,30 +2765,32 @@
       <c r="I4" s="5">
         <v>6</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
+      <c r="J4" s="19">
+        <v>4</v>
+      </c>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
       <c r="AE4" s="8">
         <f>B4-(SUM(C4:AD4))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.35">
@@ -2800,30 +2821,32 @@
       <c r="I5" s="5">
         <v>2</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
+      <c r="J5" s="19">
+        <v>4</v>
+      </c>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
       <c r="AE5" s="8">
         <f>B5-(SUM(C5:AD5))</f>
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.35">
@@ -2854,16 +2877,27 @@
       <c r="I6" s="6">
         <v>0</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="9"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="21"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="21"/>
+      <c r="AC6" s="21"/>
+      <c r="AD6" s="21"/>
       <c r="AE6" s="17">
         <f>B6-(SUM(C6:AD6))</f>
         <v>10</v>
@@ -3118,7 +3152,7 @@
       </c>
       <c r="J11" s="15">
         <f>SUM(J2:J6)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K11" s="15">
         <f t="shared" ref="K11:AD11" si="2">SUM(K2:K6)</f>
@@ -3239,87 +3273,87 @@
       </c>
       <c r="J12" s="14">
         <f t="shared" ref="J12" si="5">I12-J11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="K12" s="14">
         <f t="shared" ref="K12" si="6">J12-K11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="L12" s="14">
         <f t="shared" ref="L12" si="7">K12-L11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="M12" s="14">
         <f t="shared" ref="M12" si="8">L12-M11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="N12" s="14">
         <f t="shared" ref="N12" si="9">M12-N11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="O12" s="14">
         <f t="shared" ref="O12" si="10">N12-O11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="P12" s="14">
         <f t="shared" ref="P12" si="11">O12-P11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="Q12" s="14">
         <f t="shared" ref="Q12" si="12">P12-Q11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="R12" s="14">
         <f t="shared" ref="R12" si="13">Q12-R11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="S12" s="14">
         <f t="shared" ref="S12" si="14">R12-S11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="T12" s="14">
         <f t="shared" ref="T12" si="15">S12-T11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="U12" s="14">
         <f t="shared" ref="U12" si="16">T12-U11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="V12" s="14">
         <f t="shared" ref="V12" si="17">U12-V11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="W12" s="14">
         <f t="shared" ref="W12" si="18">V12-W11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="X12" s="14">
         <f t="shared" ref="X12" si="19">W12-X11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="Y12" s="14">
         <f t="shared" ref="Y12" si="20">X12-Y11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="Z12" s="14">
         <f t="shared" ref="Z12" si="21">Y12-Z11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AA12" s="14">
         <f t="shared" ref="AA12" si="22">Z12-AA11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AB12" s="14">
         <f t="shared" ref="AB12" si="23">AA12-AB11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AC12" s="14">
         <f t="shared" ref="AC12" si="24">AB12-AC11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AD12" s="14">
         <f t="shared" ref="AD12" si="25">AC12-AD11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Animation for main page
</commit_message>
<xml_diff>
--- a/doc/organisation/Burndown Chart/Sprint 4.xlsx
+++ b/doc/organisation/Burndown Chart/Sprint 4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patigny.nicolas\AndroidStudioProjects\BSN_2024\doc\organisation\Burndown Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662941F9-3C1B-45DF-898F-EEB66D6F5ADE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F598712F-98AA-444C-BAA8-329ECB520737}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Initial Estimate</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>US#4 SQL:Mika+Karim+Al</t>
-  </si>
-  <si>
-    <t>US#5 API:Al</t>
   </si>
   <si>
     <t>0.5</t>
@@ -560,88 +557,88 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="1">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.0714285714285716</c:v>
+                  <c:v>1.6428571428571428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -790,7 +787,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -802,7 +799,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -814,7 +811,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -832,7 +829,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1028,91 +1025,91 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>25</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>25</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>25</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>25</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>25</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>25</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>25</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1255,91 +1252,91 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>58</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.928571428571431</c:v>
+                  <c:v>44.357142857142854</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.857142857142861</c:v>
+                  <c:v>42.714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51.785714285714292</c:v>
+                  <c:v>41.071428571428562</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49.714285714285722</c:v>
+                  <c:v>39.428571428571416</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47.642857142857153</c:v>
+                  <c:v>37.78571428571427</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45.571428571428584</c:v>
+                  <c:v>36.142857142857125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43.500000000000014</c:v>
+                  <c:v>34.499999999999979</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41.428571428571445</c:v>
+                  <c:v>32.857142857142833</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39.357142857142875</c:v>
+                  <c:v>31.21428571428569</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>37.285714285714306</c:v>
+                  <c:v>29.571428571428548</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>35.214285714285737</c:v>
+                  <c:v>27.928571428571406</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>33.142857142857167</c:v>
+                  <c:v>26.285714285714263</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>31.071428571428594</c:v>
+                  <c:v>24.642857142857121</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29.000000000000021</c:v>
+                  <c:v>22.999999999999979</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26.928571428571448</c:v>
+                  <c:v>21.357142857142836</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>24.857142857142875</c:v>
+                  <c:v>19.714285714285694</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22.785714285714302</c:v>
+                  <c:v>18.071428571428552</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20.71428571428573</c:v>
+                  <c:v>16.428571428571409</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>18.642857142857157</c:v>
+                  <c:v>14.785714285714267</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16.571428571428584</c:v>
+                  <c:v>13.142857142857125</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>14.500000000000012</c:v>
+                  <c:v>11.499999999999982</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>12.428571428571441</c:v>
+                  <c:v>9.8571428571428399</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10.35714285714287</c:v>
+                  <c:v>8.2142857142856975</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.2857142857142989</c:v>
+                  <c:v>6.5714285714285552</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.2142857142857277</c:v>
+                  <c:v>4.9285714285714128</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.1428571428571566</c:v>
+                  <c:v>3.28571428571427</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.0714285714285849</c:v>
+                  <c:v>1.6428571428571273</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.3322676295501878E-14</c:v>
+                  <c:v>-1.5543122344752192E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2511,26 +2508,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB23A665-88C7-4222-B918-AB1BED6AEF55}">
   <dimension ref="A1:AN13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="7.08984375" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" customWidth="1"/>
-    <col min="7" max="7" width="7.54296875" customWidth="1"/>
-    <col min="8" max="19" width="7.26953125" customWidth="1"/>
-    <col min="20" max="20" width="10.08984375" customWidth="1"/>
-    <col min="21" max="21" width="11.453125" customWidth="1"/>
-    <col min="22" max="22" width="8.81640625" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="19" width="7.28515625" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -2625,7 +2622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -2654,34 +2651,74 @@
         <v>5</v>
       </c>
       <c r="J2" s="19">
-        <v>2</v>
-      </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="K2" s="19">
+        <v>0</v>
+      </c>
+      <c r="L2" s="19">
+        <v>0</v>
+      </c>
+      <c r="M2" s="19">
+        <v>0</v>
+      </c>
+      <c r="N2" s="19">
+        <v>1</v>
+      </c>
+      <c r="O2" s="19">
+        <v>0</v>
+      </c>
+      <c r="P2" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="19">
+        <v>0</v>
+      </c>
+      <c r="R2" s="19">
+        <v>0</v>
+      </c>
+      <c r="S2" s="19">
+        <v>0</v>
+      </c>
+      <c r="T2" s="19">
+        <v>1</v>
+      </c>
+      <c r="U2" s="19">
+        <v>0</v>
+      </c>
+      <c r="V2" s="19">
+        <v>0</v>
+      </c>
+      <c r="W2" s="19">
+        <v>0</v>
+      </c>
+      <c r="X2" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="19">
+        <v>0</v>
+      </c>
       <c r="AE2" s="8">
         <f>B2-(SUM(C2:AD2))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -2710,34 +2747,74 @@
         <v>2</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
-      <c r="Z3" s="18"/>
-      <c r="AA3" s="18"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="18"/>
-      <c r="AD3" s="18"/>
+        <v>41</v>
+      </c>
+      <c r="K3" s="18">
+        <v>0</v>
+      </c>
+      <c r="L3" s="18">
+        <v>0</v>
+      </c>
+      <c r="M3" s="18">
+        <v>0</v>
+      </c>
+      <c r="N3" s="18">
+        <v>0</v>
+      </c>
+      <c r="O3" s="18">
+        <v>0</v>
+      </c>
+      <c r="P3" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="18">
+        <v>0</v>
+      </c>
+      <c r="R3" s="18">
+        <v>0</v>
+      </c>
+      <c r="S3" s="18">
+        <v>0</v>
+      </c>
+      <c r="T3" s="18">
+        <v>0</v>
+      </c>
+      <c r="U3" s="18">
+        <v>0</v>
+      </c>
+      <c r="V3" s="18">
+        <v>0</v>
+      </c>
+      <c r="W3" s="18">
+        <v>0</v>
+      </c>
+      <c r="X3" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="18">
+        <v>0</v>
+      </c>
       <c r="AE3" s="9">
         <f>B3-(SUM(C3:AD3))</f>
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -2768,32 +2845,72 @@
       <c r="J4" s="19">
         <v>4</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
+      <c r="K4" s="19">
+        <v>0</v>
+      </c>
+      <c r="L4" s="19">
+        <v>0</v>
+      </c>
+      <c r="M4" s="19">
+        <v>0</v>
+      </c>
+      <c r="N4" s="19">
+        <v>0</v>
+      </c>
+      <c r="O4" s="19">
+        <v>0</v>
+      </c>
+      <c r="P4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>0</v>
+      </c>
+      <c r="R4" s="19">
+        <v>0</v>
+      </c>
+      <c r="S4" s="19">
+        <v>0</v>
+      </c>
+      <c r="T4" s="19">
+        <v>0</v>
+      </c>
+      <c r="U4" s="19">
+        <v>0</v>
+      </c>
+      <c r="V4" s="19">
+        <v>0</v>
+      </c>
+      <c r="W4" s="19">
+        <v>0</v>
+      </c>
+      <c r="X4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="19">
+        <v>0</v>
+      </c>
       <c r="AE4" s="8">
         <f>B4-(SUM(C4:AD4))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
@@ -2824,59 +2941,81 @@
       <c r="J5" s="19">
         <v>4</v>
       </c>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19"/>
-      <c r="AA5" s="19"/>
-      <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
+      <c r="K5" s="19">
+        <v>0</v>
+      </c>
+      <c r="L5" s="19">
+        <v>0</v>
+      </c>
+      <c r="M5" s="19">
+        <v>0</v>
+      </c>
+      <c r="N5" s="19">
+        <v>2</v>
+      </c>
+      <c r="O5" s="19">
+        <v>0</v>
+      </c>
+      <c r="P5" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>0</v>
+      </c>
+      <c r="R5" s="19">
+        <v>0</v>
+      </c>
+      <c r="S5" s="19">
+        <v>0</v>
+      </c>
+      <c r="T5" s="19">
+        <v>1</v>
+      </c>
+      <c r="U5" s="19">
+        <v>0</v>
+      </c>
+      <c r="V5" s="19">
+        <v>0</v>
+      </c>
+      <c r="W5" s="19">
+        <v>0</v>
+      </c>
+      <c r="X5" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="19">
+        <v>0</v>
+      </c>
       <c r="AE5" s="8">
         <f>B5-(SUM(C5:AD5))</f>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="6">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>2</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0</v>
-      </c>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
@@ -2900,14 +3039,14 @@
       <c r="AD6" s="21"/>
       <c r="AE6" s="17">
         <f>B6-(SUM(C6:AD6))</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AN6" s="9">
         <f>B6-(SUM(C6:AM6))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -2999,125 +3138,125 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="14">
         <f>SUM(B2:B6)/28</f>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="D10" s="14">
         <f t="shared" ref="D10:AD10" si="0">SUM($B$2:$B$6)/28</f>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="E10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="F10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="G10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="H10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="I10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="J10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="K10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="L10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="M10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="N10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="O10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="P10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="Q10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="R10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="S10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="T10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="U10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="V10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="W10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="X10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="Y10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="Z10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="AA10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="AB10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="AC10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
       <c r="AD10" s="14">
         <f t="shared" si="0"/>
-        <v>2.0714285714285716</v>
+        <v>1.6428571428571428</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
@@ -3136,7 +3275,7 @@
       </c>
       <c r="F11" s="15">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G11" s="15">
         <f t="shared" si="1"/>
@@ -3152,7 +3291,7 @@
       </c>
       <c r="J11" s="15">
         <f>SUM(J2:J6)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K11" s="15">
         <f t="shared" ref="K11:AD11" si="2">SUM(K2:K6)</f>
@@ -3168,7 +3307,7 @@
       </c>
       <c r="N11" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O11" s="15">
         <f t="shared" si="2"/>
@@ -3192,7 +3331,7 @@
       </c>
       <c r="T11" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U11" s="15">
         <f t="shared" si="2"/>
@@ -3235,246 +3374,246 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="5">
         <f>SUM(B2:B6)</f>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C12" s="14">
         <f>B12-C11</f>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D12" s="14">
         <f t="shared" ref="D12:H12" si="3">C12-D11</f>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E12" s="14">
         <f t="shared" si="3"/>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F12" s="14">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G12" s="14">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H12" s="14">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I12" s="14">
         <f t="shared" ref="I12" si="4">H12-I11</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J12" s="14">
         <f t="shared" ref="J12" si="5">I12-J11</f>
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="K12" s="14">
         <f t="shared" ref="K12" si="6">J12-K11</f>
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="L12" s="14">
         <f t="shared" ref="L12" si="7">K12-L11</f>
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="M12" s="14">
         <f t="shared" ref="M12" si="8">L12-M11</f>
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="N12" s="14">
         <f t="shared" ref="N12" si="9">M12-N11</f>
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="O12" s="14">
         <f t="shared" ref="O12" si="10">N12-O11</f>
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="P12" s="14">
         <f t="shared" ref="P12" si="11">O12-P11</f>
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="Q12" s="14">
         <f t="shared" ref="Q12" si="12">P12-Q11</f>
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="R12" s="14">
         <f t="shared" ref="R12" si="13">Q12-R11</f>
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="S12" s="14">
         <f t="shared" ref="S12" si="14">R12-S11</f>
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="T12" s="14">
         <f t="shared" ref="T12" si="15">S12-T11</f>
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="U12" s="14">
         <f t="shared" ref="U12" si="16">T12-U11</f>
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="V12" s="14">
         <f t="shared" ref="V12" si="17">U12-V11</f>
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="W12" s="14">
         <f t="shared" ref="W12" si="18">V12-W11</f>
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="X12" s="14">
         <f t="shared" ref="X12" si="19">W12-X11</f>
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="Y12" s="14">
         <f t="shared" ref="Y12" si="20">X12-Y11</f>
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="Z12" s="14">
         <f t="shared" ref="Z12" si="21">Y12-Z11</f>
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="AA12" s="14">
         <f t="shared" ref="AA12" si="22">Z12-AA11</f>
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="AB12" s="14">
         <f t="shared" ref="AB12" si="23">AA12-AB11</f>
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="AC12" s="14">
         <f t="shared" ref="AC12" si="24">AB12-AC11</f>
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="AD12" s="14">
         <f t="shared" ref="AD12" si="25">AC12-AD11</f>
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="1">
         <f>SUM(B2:B6)</f>
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C13" s="16">
         <f>B13-C10</f>
-        <v>55.928571428571431</v>
+        <v>44.357142857142854</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" ref="D13:H13" si="26">C13-D10</f>
-        <v>53.857142857142861</v>
+        <v>42.714285714285708</v>
       </c>
       <c r="E13" s="16">
         <f t="shared" si="26"/>
-        <v>51.785714285714292</v>
+        <v>41.071428571428562</v>
       </c>
       <c r="F13" s="16">
         <f t="shared" si="26"/>
-        <v>49.714285714285722</v>
+        <v>39.428571428571416</v>
       </c>
       <c r="G13" s="16">
         <f t="shared" si="26"/>
-        <v>47.642857142857153</v>
+        <v>37.78571428571427</v>
       </c>
       <c r="H13" s="16">
         <f t="shared" si="26"/>
-        <v>45.571428571428584</v>
+        <v>36.142857142857125</v>
       </c>
       <c r="I13" s="16">
         <f t="shared" ref="I13" si="27">H13-I10</f>
-        <v>43.500000000000014</v>
+        <v>34.499999999999979</v>
       </c>
       <c r="J13" s="16">
         <f t="shared" ref="J13" si="28">I13-J10</f>
-        <v>41.428571428571445</v>
+        <v>32.857142857142833</v>
       </c>
       <c r="K13" s="16">
         <f t="shared" ref="K13" si="29">J13-K10</f>
-        <v>39.357142857142875</v>
+        <v>31.21428571428569</v>
       </c>
       <c r="L13" s="16">
         <f t="shared" ref="L13" si="30">K13-L10</f>
-        <v>37.285714285714306</v>
+        <v>29.571428571428548</v>
       </c>
       <c r="M13" s="16">
         <f t="shared" ref="M13" si="31">L13-M10</f>
-        <v>35.214285714285737</v>
+        <v>27.928571428571406</v>
       </c>
       <c r="N13" s="16">
         <f t="shared" ref="N13" si="32">M13-N10</f>
-        <v>33.142857142857167</v>
+        <v>26.285714285714263</v>
       </c>
       <c r="O13" s="16">
         <f t="shared" ref="O13" si="33">N13-O10</f>
-        <v>31.071428571428594</v>
+        <v>24.642857142857121</v>
       </c>
       <c r="P13" s="16">
         <f t="shared" ref="P13" si="34">O13-P10</f>
-        <v>29.000000000000021</v>
+        <v>22.999999999999979</v>
       </c>
       <c r="Q13" s="16">
         <f t="shared" ref="Q13" si="35">P13-Q10</f>
-        <v>26.928571428571448</v>
+        <v>21.357142857142836</v>
       </c>
       <c r="R13" s="16">
         <f t="shared" ref="R13" si="36">Q13-R10</f>
-        <v>24.857142857142875</v>
+        <v>19.714285714285694</v>
       </c>
       <c r="S13" s="16">
         <f t="shared" ref="S13" si="37">R13-S10</f>
-        <v>22.785714285714302</v>
+        <v>18.071428571428552</v>
       </c>
       <c r="T13" s="16">
         <f t="shared" ref="T13" si="38">S13-T10</f>
-        <v>20.71428571428573</v>
+        <v>16.428571428571409</v>
       </c>
       <c r="U13" s="16">
         <f t="shared" ref="U13" si="39">T13-U10</f>
-        <v>18.642857142857157</v>
+        <v>14.785714285714267</v>
       </c>
       <c r="V13" s="16">
         <f t="shared" ref="V13" si="40">U13-V10</f>
-        <v>16.571428571428584</v>
+        <v>13.142857142857125</v>
       </c>
       <c r="W13" s="16">
         <f t="shared" ref="W13" si="41">V13-W10</f>
-        <v>14.500000000000012</v>
+        <v>11.499999999999982</v>
       </c>
       <c r="X13" s="16">
         <f t="shared" ref="X13" si="42">W13-X10</f>
-        <v>12.428571428571441</v>
+        <v>9.8571428571428399</v>
       </c>
       <c r="Y13" s="16">
         <f t="shared" ref="Y13" si="43">X13-Y10</f>
-        <v>10.35714285714287</v>
+        <v>8.2142857142856975</v>
       </c>
       <c r="Z13" s="16">
         <f t="shared" ref="Z13" si="44">Y13-Z10</f>
-        <v>8.2857142857142989</v>
+        <v>6.5714285714285552</v>
       </c>
       <c r="AA13" s="16">
         <f t="shared" ref="AA13" si="45">Z13-AA10</f>
-        <v>6.2142857142857277</v>
+        <v>4.9285714285714128</v>
       </c>
       <c r="AB13" s="16">
         <f t="shared" ref="AB13" si="46">AA13-AB10</f>
-        <v>4.1428571428571566</v>
+        <v>3.28571428571427</v>
       </c>
       <c r="AC13" s="16">
         <f t="shared" ref="AC13" si="47">AB13-AC10</f>
-        <v>2.0714285714285849</v>
+        <v>1.6428571428571273</v>
       </c>
       <c r="AD13" s="16">
         <f t="shared" ref="AD13" si="48">AC13-AD10</f>
-        <v>1.3322676295501878E-14</v>
+        <v>-1.5543122344752192E-14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>